<commit_message>
updated to automatically generate opool file
</commit_message>
<xml_diff>
--- a/test/output/P4P6_mutate_rescue_library.xlsx
+++ b/test/output/P4P6_mutate_rescue_library.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="27..43" sheetId="1" r:id="rId1"/>
+    <sheet name="All Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>Sequence</t>
   </si>
@@ -37,6 +38,9 @@
     <t>Edit Distance</t>
   </si>
   <si>
+    <t>Helix</t>
+  </si>
+  <si>
     <t>GGCGTCGAGTAGACGCC</t>
   </si>
   <si>
@@ -49,10 +53,10 @@
     <t>CTGCGGGAGTACCGCAG</t>
   </si>
   <si>
-    <t>CGGTCGGAGTACGCCGA</t>
-  </si>
-  <si>
-    <t>CGGGTCGAGTAAGCCCG</t>
+    <t>CTGGCGGAGTACCACGG</t>
+  </si>
+  <si>
+    <t>TGCCGGGAGTACCGGCA</t>
   </si>
   <si>
     <t>((((((.....))))))</t>
@@ -61,9 +65,6 @@
     <t>.................</t>
   </si>
   <si>
-    <t>(((((.......)))))</t>
-  </si>
-  <si>
     <t>WT</t>
   </si>
   <si>
@@ -80,6 +81,9 @@
   </si>
   <si>
     <t>Stochastic Helix Rescue</t>
+  </si>
+  <si>
+    <t>[[0, 16], [1, 15], [2, 14], [3, 13], [4, 12], [5, 11]]</t>
   </si>
 </sst>
 </file>
@@ -444,6 +448,189 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>-0.17</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>-0.17</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>5.2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>-0.17</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>5.19</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,16 +652,19 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -483,15 +673,15 @@
         <v>5.93</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -508,16 +698,19 @@
       <c r="H3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -534,16 +727,19 @@
       <c r="H4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -560,16 +756,19 @@
       <c r="H5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -584,33 +783,39 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7">
-        <v>3.1</v>
+        <v>5.19</v>
       </c>
       <c r="F7">
-        <v>0.1666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>